<commit_message>
Added signal description document for CAN protocol. Updated CAN protocol.
</commit_message>
<xml_diff>
--- a/docs/CAN_Protocol_2017.xlsx
+++ b/docs/CAN_Protocol_2017.xlsx
@@ -237,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -330,11 +330,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -348,52 +377,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -402,13 +392,61 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -416,9 +454,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -451,6 +486,9 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -465,11 +503,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:C16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4" headerRowCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:C16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Node Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Acronym" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" name="Node Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Acronym" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -741,7 +779,7 @@
   <dimension ref="A1:AD51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="N8" sqref="N8:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,60 +798,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -824,33 +862,33 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="27">
+      <c r="I3" s="9">
         <v>7</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="9">
         <v>6</v>
       </c>
-      <c r="K3" s="27">
+      <c r="K3" s="9">
         <v>5</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="9">
         <v>4</v>
       </c>
-      <c r="M3" s="27">
+      <c r="M3" s="9">
         <v>3</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="9">
         <v>2</v>
       </c>
-      <c r="O3" s="27">
+      <c r="O3" s="9">
         <v>1</v>
       </c>
-      <c r="P3" s="27">
+      <c r="P3" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -859,7 +897,7 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -879,21 +917,21 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="18"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -903,12 +941,12 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -917,7 +955,7 @@
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -937,21 +975,21 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="22"/>
+      <c r="P6" s="25"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -961,12 +999,12 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="24"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="27"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -975,7 +1013,7 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="18" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -995,21 +1033,21 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="13" t="s">
+      <c r="N8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="O8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="18"/>
+      <c r="P8" s="21"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1019,17 +1057,17 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="20"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="31"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1039,12 +1077,12 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1053,7 +1091,7 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="19" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1075,17 +1113,17 @@
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="11" t="s">
+      <c r="P11" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -1097,10 +1135,10 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="12"/>
+      <c r="P12" s="15"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1109,7 +1147,7 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="18" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1131,17 +1169,17 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="16" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1153,10 +1191,10 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="14"/>
+      <c r="P14" s="17"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1165,7 +1203,7 @@
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="19" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="8"/>
@@ -1185,17 +1223,17 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -1207,7 +1245,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="12"/>
+      <c r="P16" s="15"/>
     </row>
     <row r="51" spans="30:30" x14ac:dyDescent="0.25">
       <c r="AD51" t="s">
@@ -1216,6 +1254,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O8:P10"/>
+    <mergeCell ref="N8:N10"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="I2:P2"/>
     <mergeCell ref="P11:P12"/>
@@ -1231,8 +1271,6 @@
     <mergeCell ref="O4:P5"/>
     <mergeCell ref="O6:P7"/>
     <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Filled in half of Test Plan
</commit_message>
<xml_diff>
--- a/docs/CAN_Protocol_2017.xlsx
+++ b/docs/CAN_Protocol_2017.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Node Name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Up/Down Status</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -386,6 +389,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -398,56 +434,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,7 +794,7 @@
   <dimension ref="A1:AD51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N10"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,24 +813,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -842,16 +857,16 @@
       <c r="H2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -888,7 +903,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -897,7 +912,7 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="27" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -917,21 +932,21 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="21"/>
+      <c r="P4" s="15"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -941,12 +956,12 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="23"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -955,7 +970,7 @@
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="28" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
@@ -975,21 +990,21 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="25"/>
+      <c r="P6" s="30"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -999,12 +1014,12 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="27"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="32"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1013,7 +1028,7 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="27" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1033,21 +1048,21 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="16" t="s">
+      <c r="N8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="21"/>
+      <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1057,17 +1072,17 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="31"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1077,12 +1092,12 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="23"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="19"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1091,7 +1106,7 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="28" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1112,18 +1127,18 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="14" t="s">
+      <c r="O11" s="35"/>
+      <c r="P11" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -1134,11 +1149,11 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="15"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1147,7 +1162,7 @@
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="27" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -1168,18 +1183,20 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="16" t="s">
+      <c r="O13" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="P13" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1190,11 +1207,11 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="17"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="22"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1203,7 +1220,7 @@
       <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="8"/>
@@ -1222,18 +1239,18 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="14" t="s">
+      <c r="O15" s="35"/>
+      <c r="P15" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -1244,8 +1261,8 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="15"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="51" spans="30:30" x14ac:dyDescent="0.25">
       <c r="AD51" t="s">
@@ -1253,12 +1270,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="O8:P10"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="I2:P2"/>
-    <mergeCell ref="P11:P12"/>
+  <mergeCells count="20">
     <mergeCell ref="P13:P14"/>
     <mergeCell ref="P15:P16"/>
     <mergeCell ref="D4:D5"/>
@@ -1271,6 +1283,14 @@
     <mergeCell ref="O4:P5"/>
     <mergeCell ref="O6:P7"/>
     <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O8:P10"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="I2:P2"/>
+    <mergeCell ref="P11:P12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>